<commit_message>
EXE Version 1 complete
</commit_message>
<xml_diff>
--- a/AQ_Budgets/5721_AQ_formatted.xlsx
+++ b/AQ_Budgets/5721_AQ_formatted.xlsx
@@ -189,6 +189,36 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="2638425" cy="1790700"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,7 +505,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -54983,5 +55013,6 @@
     <mergeCell ref="A2048:C2048"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>